<commit_message>
Finish some missing services, correct query method and other few changes
</commit_message>
<xml_diff>
--- a/src/main/resources/CAMPAIGN.xlsx
+++ b/src/main/resources/CAMPAIGN.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="18">
   <si>
     <t>CUSTOMER_NUMBER</t>
   </si>
@@ -56,98 +56,35 @@
     <t>TERM_AND_CONDITIONS_LINK</t>
   </si>
   <si>
-    <t>dev@test.com</t>
+    <t>prueba@prueba.com</t>
   </si>
   <si>
-    <t>PROMOCION NETFLIX</t>
+    <t>PROMOCION AMAZON</t>
   </si>
   <si>
-    <t>CONTRATA NETFLIX Y RECIBE 10% DE DESCUENTO</t>
+    <t>OFERTA AMAZON PRODUCTO</t>
   </si>
   <si>
-    <t>NETFLIX001</t>
+    <t>GRATIS PRODUCTO AMZ</t>
   </si>
   <si>
-    <t>DESCUENTO</t>
+    <t>2022-05-01</t>
   </si>
   <si>
-    <t>2022-05-05</t>
+    <t>2022-06-01</t>
   </si>
   <si>
-    <t>2022-06-05</t>
+    <t>https://www.terminos-y-condiciones/amz/promo/2022-05/info.html</t>
   </si>
   <si>
-    <t>https://www.terminos-y-condiciones/netflix/promo/2022-05/info.html</t>
-  </si>
-  <si>
-    <t>NETFLIX002</t>
-  </si>
-  <si>
-    <t>NETFLIX003</t>
-  </si>
-  <si>
-    <t>NETFLIX004</t>
-  </si>
-  <si>
-    <t>NETFLIX005</t>
-  </si>
-  <si>
-    <t>NETFLIX006</t>
-  </si>
-  <si>
-    <t>NETFLIX007</t>
-  </si>
-  <si>
-    <t>NETFLIX008</t>
-  </si>
-  <si>
-    <t>2022-05-06</t>
-  </si>
-  <si>
-    <t>2022-06-06</t>
-  </si>
-  <si>
-    <t>2022-05-07</t>
-  </si>
-  <si>
-    <t>2022-06-07</t>
-  </si>
-  <si>
-    <t>2022-05-08</t>
-  </si>
-  <si>
-    <t>2022-06-08</t>
-  </si>
-  <si>
-    <t>2022-05-09</t>
-  </si>
-  <si>
-    <t>2022-06-09</t>
-  </si>
-  <si>
-    <t>2022-05-10</t>
-  </si>
-  <si>
-    <t>2022-06-10</t>
-  </si>
-  <si>
-    <t>2022-05-11</t>
-  </si>
-  <si>
-    <t>2022-06-11</t>
-  </si>
-  <si>
-    <t>2022-05-12</t>
-  </si>
-  <si>
-    <t>2022-06-12</t>
+    <t>AMZ20220501</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -174,13 +111,6 @@
       <name val="Cambria"/>
       <family val="1"/>
     </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="10"/>
-      <name val="Cambria"/>
-      <family val="1"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -203,7 +133,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -211,7 +141,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -497,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -512,8 +441,8 @@
     <col min="5" max="5" width="20.140625" style="4" customWidth="1"/>
     <col min="6" max="6" width="17.7109375" style="4" customWidth="1"/>
     <col min="7" max="7" width="16.140625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" style="6" customWidth="1"/>
-    <col min="9" max="9" width="14" style="6" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" style="5" customWidth="1"/>
+    <col min="9" max="9" width="14" style="5" customWidth="1"/>
     <col min="10" max="10" width="64.42578125" style="4" customWidth="1"/>
     <col min="11" max="16384" width="11.42578125" style="4"/>
   </cols>
@@ -540,10 +469,10 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="6" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
@@ -553,9 +482,9 @@
     </row>
     <row r="2" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5" t="s">
+        <v>10000</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -565,29 +494,29 @@
         <v>12</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F2" s="4">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5" t="s">
+        <v>10001</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -597,29 +526,29 @@
         <v>12</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F3" s="4">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5" t="s">
+        <v>10002</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -629,29 +558,29 @@
         <v>12</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F4" s="4">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5" t="s">
+        <v>10003</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -661,29 +590,29 @@
         <v>12</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F5" s="4">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>26</v>
+        <v>13</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
-        <v>5</v>
-      </c>
-      <c r="B6" s="5" t="s">
+        <v>10004</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -693,29 +622,29 @@
         <v>12</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F6" s="4">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>28</v>
+        <v>13</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
-        <v>6</v>
-      </c>
-      <c r="B7" s="5" t="s">
+        <v>10005</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -725,29 +654,29 @@
         <v>12</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F7" s="4">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>30</v>
+        <v>13</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
-        <v>7</v>
-      </c>
-      <c r="B8" s="5" t="s">
+        <v>10006</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -757,29 +686,29 @@
         <v>12</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F8" s="4">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>32</v>
+        <v>13</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
-        <v>8</v>
-      </c>
-      <c r="B9" s="5" t="s">
+        <v>10007</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="4" t="s">
@@ -789,29 +718,29 @@
         <v>12</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="F9" s="4">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>34</v>
+        <v>13</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
-        <v>9</v>
-      </c>
-      <c r="B10" s="5" t="s">
+        <v>10008</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C10" s="4" t="s">
@@ -821,29 +750,29 @@
         <v>12</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F10" s="4">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>36</v>
+        <v>13</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
-        <v>10</v>
-      </c>
-      <c r="B11" s="5" t="s">
+        <v>10009</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -853,40 +782,1346 @@
         <v>12</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="F11" s="4">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>38</v>
+        <v>13</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>10010</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="4">
+        <v>0</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>10011</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="4">
+        <v>0</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>10012</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" s="4">
+        <v>0</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>10013</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" s="4">
+        <v>0</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>10014</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" s="4">
+        <v>0</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>10015</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" s="4">
+        <v>0</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>10016</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" s="4">
+        <v>0</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>10017</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" s="4">
+        <v>0</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>10018</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" s="4">
+        <v>0</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>10019</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" s="4">
+        <v>0</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>10020</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" s="4">
+        <v>0</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>10021</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" s="4">
+        <v>0</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>10022</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F24" s="4">
+        <v>0</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>10023</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F25" s="4">
+        <v>0</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>10024</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F26" s="4">
+        <v>0</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>10025</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F27" s="4">
+        <v>0</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <v>10026</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F28" s="4">
+        <v>0</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <v>10027</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F29" s="4">
+        <v>0</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <v>10028</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F30" s="4">
+        <v>0</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J30" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <v>10029</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F31" s="4">
+        <v>0</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J31" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A32" s="4">
+        <v>10030</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F32" s="4">
+        <v>0</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J32" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
+        <v>10031</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F33" s="4">
+        <v>0</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I33" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J33" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
+        <v>10032</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F34" s="4">
+        <v>0</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I34" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J34" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
+        <v>10033</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F35" s="4">
+        <v>0</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I35" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J35" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
+        <v>10034</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F36" s="4">
+        <v>0</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I36" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J36" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A37" s="4">
+        <v>10035</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F37" s="4">
+        <v>0</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I37" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J37" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A38" s="4">
+        <v>10036</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F38" s="4">
+        <v>0</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I38" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J38" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A39" s="4">
+        <v>10037</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F39" s="4">
+        <v>0</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I39" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J39" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A40" s="4">
+        <v>10038</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F40" s="4">
+        <v>0</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I40" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J40" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A41" s="4">
+        <v>10039</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F41" s="4">
+        <v>0</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H41" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I41" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J41" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A42" s="4">
+        <v>10040</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F42" s="4">
+        <v>0</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H42" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I42" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J42" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A43" s="4">
+        <v>10041</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F43" s="4">
+        <v>0</v>
+      </c>
+      <c r="G43" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H43" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I43" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J43" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A44" s="4">
+        <v>10042</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F44" s="4">
+        <v>0</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H44" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I44" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J44" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A45" s="4">
+        <v>10043</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F45" s="4">
+        <v>0</v>
+      </c>
+      <c r="G45" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H45" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I45" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J45" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A46" s="4">
+        <v>10044</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F46" s="4">
+        <v>0</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H46" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I46" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J46" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A47" s="4">
+        <v>10045</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F47" s="4">
+        <v>0</v>
+      </c>
+      <c r="G47" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H47" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I47" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J47" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A48" s="4">
+        <v>10046</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F48" s="4">
+        <v>0</v>
+      </c>
+      <c r="G48" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H48" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I48" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J48" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A49" s="4">
+        <v>10047</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F49" s="4">
+        <v>0</v>
+      </c>
+      <c r="G49" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H49" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I49" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J49" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A50" s="4">
+        <v>10048</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F50" s="4">
+        <v>0</v>
+      </c>
+      <c r="G50" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H50" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I50" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J50" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A51" s="4">
+        <v>10049</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F51" s="4">
+        <v>0</v>
+      </c>
+      <c r="G51" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H51" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I51" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J51" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A52" s="4">
+        <v>10050</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F52" s="4">
+        <v>0</v>
+      </c>
+      <c r="G52" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H52" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I52" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J52" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3:B4" r:id="rId2" display="dev@test.com"/>
-    <hyperlink ref="J2" r:id="rId3"/>
-    <hyperlink ref="J3:J4" r:id="rId4" display="https://www.terminos-y-condiciones/netflix/promo/2022-05/info.html"/>
-    <hyperlink ref="B5:B11" r:id="rId5" display="dev@test.com"/>
-    <hyperlink ref="J5" r:id="rId6"/>
-    <hyperlink ref="J6" r:id="rId7"/>
-    <hyperlink ref="J7" r:id="rId8"/>
-    <hyperlink ref="J8" r:id="rId9"/>
-    <hyperlink ref="J9" r:id="rId10"/>
-    <hyperlink ref="J10" r:id="rId11"/>
-    <hyperlink ref="J11" r:id="rId12"/>
+    <hyperlink ref="J2" r:id="rId1"/>
+    <hyperlink ref="B5:B11" r:id="rId2" display="dev@test.com"/>
+    <hyperlink ref="B11" r:id="rId3"/>
+    <hyperlink ref="B2:B10" r:id="rId4" display="dev@test.com"/>
+    <hyperlink ref="B12:B52" r:id="rId5" display="dev@test.com"/>
+    <hyperlink ref="J3:J52" r:id="rId6" display="https://www.terminos-y-condiciones/amz/promo/2022-05/info.html"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId13"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>